<commit_message>
Many additions of code and notebooks.
</commit_message>
<xml_diff>
--- a/data/fluorimeter/Comparison_RUsilatrane_surfaces.xlsx
+++ b/data/fluorimeter/Comparison_RUsilatrane_surfaces.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10313"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jj/JuliaProjects/LaserLab/data/fluorimeter/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C5FE0E1B-CFB5-AB4E-A869-B82CB62EBF8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E8D2FE27-F89E-1B49-B9F0-85ED3C120949}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3980" yWindow="1340" windowWidth="41640" windowHeight="22320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3460" yWindow="1620" windowWidth="41000" windowHeight="19100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Comparison_RUsilatrane_surfaces" sheetId="1" r:id="rId1"/>
@@ -32912,18 +32912,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I275"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34:F275"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="M34" sqref="M34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="28" customWidth="1"/>
-    <col min="3" max="3" width="38.83203125" customWidth="1"/>
-    <col min="4" max="4" width="39" customWidth="1"/>
-    <col min="5" max="5" width="46" customWidth="1"/>
-    <col min="6" max="6" width="41.5" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">

</xml_diff>